<commit_message>
feat: correção de bugs e melhorias no código, adição da opção de executar localmente via streamlit
</commit_message>
<xml_diff>
--- a/resultados_permanente_xm.xlsx
+++ b/resultados_permanente_xm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,26 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-434.1756038345169</v>
+        <v>-356.4000064140148</v>
       </c>
       <c r="B2" t="n">
-        <v>8683.512000000001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>-461.0386967384126</v>
-      </c>
-      <c r="B3" t="n">
-        <v>9220.773999999999</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>-361.0931867508247</v>
-      </c>
-      <c r="B4" t="n">
-        <v>7221.864</v>
+        <v>7128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: atualizar arquivos de resultados e ajustar funções para processamento de dados
</commit_message>
<xml_diff>
--- a/resultados_permanente_xm.xlsx
+++ b/resultados_permanente_xm.xlsx
@@ -447,10 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-356.4000064140148</v>
+        <v>-342.771076148835</v>
       </c>
       <c r="B2" t="n">
-        <v>7128</v>
+        <v>6855.422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>